<commit_message>
Prepare worker for DB IO
</commit_message>
<xml_diff>
--- a/docs/2_CAND_Modele_Planning_2024.xlsx
+++ b/docs/2_CAND_Modele_Planning_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6E10B6-B4D3-4731-BBF9-EDEF03CC4447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1F835F-FDA6-463D-BEE2-468E99316788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="8" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="60">
   <si>
     <t>Tâches</t>
   </si>
@@ -1653,8 +1653,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>126</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
+      <xdr:col>130</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
@@ -1671,8 +1671,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3981447" y="1038225"/>
-          <a:ext cx="18126077" cy="6067425"/>
+          <a:off x="4238622" y="1038225"/>
+          <a:ext cx="18688053" cy="6391275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2081,10 +2081,10 @@
   <dimension ref="A1:GW44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="DG8" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="CO8" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="DZ24" sqref="DZ24"/>
+      <selection pane="bottomRight" activeCell="DR14" sqref="DR14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4511,9 +4511,7 @@
       <c r="DN10" s="14"/>
       <c r="DO10" s="14"/>
       <c r="DP10" s="32"/>
-      <c r="DQ10" s="32" t="s">
-        <v>28</v>
-      </c>
+      <c r="DQ10" s="32"/>
       <c r="DR10" s="14"/>
       <c r="DS10" s="15"/>
       <c r="DT10" s="13"/>
@@ -4726,7 +4724,9 @@
       <c r="DN11" s="14"/>
       <c r="DO11" s="14"/>
       <c r="DP11" s="32"/>
-      <c r="DQ11" s="14"/>
+      <c r="DQ11" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="DR11" s="14"/>
       <c r="DS11" s="15"/>
       <c r="DT11" s="13"/>
@@ -4941,7 +4941,9 @@
       <c r="DN12" s="14"/>
       <c r="DO12" s="14"/>
       <c r="DP12" s="14"/>
-      <c r="DQ12" s="14"/>
+      <c r="DQ12" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="DR12" s="14"/>
       <c r="DS12" s="15"/>
       <c r="DT12" s="13"/>
@@ -5160,7 +5162,9 @@
       <c r="DN13" s="14"/>
       <c r="DO13" s="14"/>
       <c r="DP13" s="14"/>
-      <c r="DQ13" s="14"/>
+      <c r="DQ13" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="DR13" s="14"/>
       <c r="DS13" s="15"/>
       <c r="DT13" s="13"/>
@@ -5370,9 +5374,7 @@
       <c r="DO14" s="14"/>
       <c r="DP14" s="14"/>
       <c r="DQ14" s="32"/>
-      <c r="DR14" s="32" t="s">
-        <v>28</v>
-      </c>
+      <c r="DR14" s="32"/>
       <c r="DS14" s="15"/>
       <c r="DT14" s="13"/>
       <c r="DU14" s="14"/>
@@ -7183,8 +7185,8 @@
       <c r="A23" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="59" t="s">
-        <v>17</v>
+      <c r="B23" s="66" t="s">
+        <v>27</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
@@ -7396,7 +7398,9 @@
       <c r="A24" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="66"/>
+      <c r="B24" s="59" t="s">
+        <v>17</v>
+      </c>
       <c r="C24" s="12"/>
       <c r="D24" s="13"/>
       <c r="E24" s="14"/>
@@ -7524,9 +7528,15 @@
       <c r="DW24" s="14"/>
       <c r="DX24" s="14"/>
       <c r="DY24" s="14"/>
-      <c r="DZ24" s="39"/>
-      <c r="EA24" s="40"/>
-      <c r="EB24" s="13"/>
+      <c r="DZ24" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="EA24" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="EB24" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="EC24" s="14"/>
       <c r="ED24" s="14"/>
       <c r="EE24" s="14"/>
@@ -7736,7 +7746,9 @@
       <c r="DZ25" s="14"/>
       <c r="EA25" s="15"/>
       <c r="EB25" s="41"/>
-      <c r="EC25" s="39"/>
+      <c r="EC25" s="39" t="s">
+        <v>28</v>
+      </c>
       <c r="ED25" s="39"/>
       <c r="EE25" s="39"/>
       <c r="EF25" s="14"/>

</xml_diff>

<commit_message>
Clean animation and add fields
- Clean framerate
- Enable "Facteur de vitesse"
- Add every vehicle settings
</commit_message>
<xml_diff>
--- a/docs/2_CAND_Modele_Planning_2024.xlsx
+++ b/docs/2_CAND_Modele_Planning_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7CCD70-5A68-446F-887E-A57E32D9432A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F96DCD-A802-4DDC-AFD0-706852C0AB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36000" yWindow="3915" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="59">
   <si>
     <r>
       <rPr>
@@ -1981,10 +1981,10 @@
   <dimension ref="A1:GW43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="DW8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="DW25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="DI1" sqref="DI1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9038,8 +9038,8 @@
       <c r="A32" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="39" t="s">
-        <v>15</v>
+      <c r="B32" s="51" t="s">
+        <v>22</v>
       </c>
       <c r="C32" s="40"/>
       <c r="D32" s="19"/>
@@ -9225,9 +9225,15 @@
       <c r="FP32" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="FQ32" s="20"/>
-      <c r="FR32" s="20"/>
-      <c r="FS32" s="20"/>
+      <c r="FQ32" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="FR32" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="FS32" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="FT32" s="20"/>
       <c r="FU32" s="20"/>
       <c r="FV32" s="20"/>
@@ -11641,7 +11647,7 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A37:B37"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6 B8:B9 B11:B13 B15:B19 B21:B36 B38 B40:B42">
+  <conditionalFormatting sqref="B6 B8:B9 B11:B13 B15:B19 B38 B40:B42 B21:B36">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",B6)))</formula>
     </cfRule>

</xml_diff>